<commit_message>
Add data collection script and update parameters for chat analysis
</commit_message>
<xml_diff>
--- a/data/results/ai_validated_chats.xlsx
+++ b/data/results/ai_validated_chats.xlsx
@@ -461,8 +461,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -625,7 +624,8 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -896,8 +896,8 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1. Нет.
-2. Нет.</t>
+          <t>1. Нет.  
+2. Да.</t>
         </is>
       </c>
     </row>
@@ -960,7 +960,8 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -991,8 +992,8 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>1. Да  
-2. Да</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1008,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -1234,7 +1235,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -1252,8 +1253,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -1411,8 +1411,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -1464,7 +1463,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1. Да  
+          <t>1. Да
 2. Да</t>
         </is>
       </c>
@@ -1879,7 +1878,8 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -2036,7 +2036,8 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -2324,7 +2325,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -2405,7 +2406,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -2541,7 +2542,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -2612,8 +2613,8 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>1. Да  
+2. Да</t>
         </is>
       </c>
     </row>
@@ -2674,7 +2675,8 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -2767,7 +2769,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -2924,7 +2926,7 @@
       <c r="C152" t="inlineStr">
         <is>
           <t>1. Нет.
-2. Нет.</t>
+2. Да.</t>
         </is>
       </c>
     </row>
@@ -2957,7 +2959,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -3268,7 +3270,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -3284,8 +3286,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -3364,8 +3365,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -3540,7 +3540,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -3591,8 +3591,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -3657,7 +3656,8 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -3704,7 +3704,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -3803,7 +3803,7 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -3919,7 +3919,8 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -4093,7 +4094,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -4142,7 +4143,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -4208,7 +4209,8 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -4225,7 +4227,7 @@
       <c r="C230" t="inlineStr">
         <is>
           <t>1. Нет.
-2. Да.</t>
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -4303,7 +4305,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -4548,7 +4550,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -4699,7 +4701,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -4889,8 +4891,8 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>1. Да  
-2. Да</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -5004,7 +5006,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -5020,8 +5022,7 @@
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -5161,7 +5162,8 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -5301,8 +5303,7 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -5381,7 +5382,8 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -5396,8 +5398,7 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -5443,8 +5444,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -5460,7 +5460,7 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -5892,7 +5892,7 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -5970,8 +5970,7 @@
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -6264,7 +6263,7 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -6295,8 +6294,7 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>1. Нет.
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -6358,7 +6356,7 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -6584,7 +6582,8 @@
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -6727,8 +6726,7 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -6948,13 +6946,7 @@
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>Пользователь: Здравствуйте! Я хотел бы узнать о статусе моего заказа.
-Оператор: Здравствуйте! Ваш заказ находится в обработке и будет отправлен в течение 3-5 рабочих дней.
-Пользователь: Почему так долго? Я ожидал, что он будет отправлен быстрее.
-Оператор: Мы прилагаем все усилия, чтобы обработать заказы как можно быстрее. Спасибо за ваше терпение.
-Пользователь: Спасибо, но я все равно разочарован.
-1. Да
-2. Да</t>
+          <t xml:space="preserve">Пользователь: </t>
         </is>
       </c>
     </row>
@@ -6969,7 +6961,8 @@
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -7000,8 +6993,7 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -7081,8 +7073,7 @@
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -7159,7 +7150,8 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -7174,7 +7166,8 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -7254,7 +7247,8 @@
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -7421,8 +7415,7 @@
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>1. Нет.
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -7438,7 +7431,8 @@
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -7453,8 +7447,7 @@
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -7502,7 +7495,7 @@
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -7615,7 +7608,7 @@
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -7652,7 +7645,7 @@
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -7755,8 +7748,7 @@
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -7872,8 +7864,7 @@
       </c>
       <c r="C456" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -7905,7 +7896,7 @@
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -8118,8 +8109,8 @@
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Да.</t>
+          <t>1. Нет.
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -8165,7 +8156,8 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -8195,7 +8187,8 @@
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -8272,8 +8265,7 @@
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -8304,7 +8296,7 @@
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -8388,7 +8380,7 @@
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -8600,7 +8592,8 @@
       </c>
       <c r="C501" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -8615,8 +8608,7 @@
       </c>
       <c r="C502" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -8883,8 +8875,8 @@
       </c>
       <c r="C518" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Да.</t>
+          <t>1. Нет.
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -9073,7 +9065,7 @@
       </c>
       <c r="C530" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -9090,7 +9082,7 @@
       </c>
       <c r="C531" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -9137,7 +9129,7 @@
       </c>
       <c r="C534" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -9170,7 +9162,7 @@
       </c>
       <c r="C536" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -9203,7 +9195,7 @@
       </c>
       <c r="C538" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -9219,8 +9211,7 @@
       </c>
       <c r="C539" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -9314,7 +9305,8 @@
       </c>
       <c r="C545" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -9460,7 +9452,15 @@
       </c>
       <c r="C554" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>Пользователь: Здравствуйте! Я хотел бы узнать о статусе моего заказа.
+ Оператор: Здравствуйте! Ваш заказ находится в обработке и будет отправлен в течение 3-5 рабочих дней.
+ Пользователь: Это слишком долго! Я ожидал, что он будет отправлен быстрее.
+ Оператор: Мы приносим извинения за задержку. Мы стараемся обработать заказы как можно быстрее.
+ Пользователь: Но я ждал уже неделю! Почему так долго?
+ Оператор: К сожалению, у нас возникли некоторые задержки из-за высокого спроса. Мы делаем все возможное, чтобы ускорить процесс.
+ Пользователь: Это не оправдание! Я не доволен вашим обслуживанием.
+1. Да
+2. Да</t>
         </is>
       </c>
     </row>
@@ -9476,7 +9476,7 @@
       </c>
       <c r="C555" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -9507,7 +9507,7 @@
       </c>
       <c r="C557" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -9556,8 +9556,7 @@
       </c>
       <c r="C560" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -9635,7 +9634,7 @@
       </c>
       <c r="C565" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -9903,8 +9902,7 @@
       </c>
       <c r="C582" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -9967,7 +9965,7 @@
       </c>
       <c r="C586" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -10030,7 +10028,7 @@
       </c>
       <c r="C590" t="inlineStr">
         <is>
-          <t>1. Нет.
+          <t>1. Нет.  
 2. Нет.</t>
         </is>
       </c>
@@ -10047,8 +10045,7 @@
       </c>
       <c r="C591" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -10204,7 +10201,8 @@
       </c>
       <c r="C601" t="inlineStr">
         <is>
-          <t>Нет.</t>
+          <t>1. Нет.  
+2. Нет.</t>
         </is>
       </c>
     </row>
@@ -10362,8 +10360,8 @@
       </c>
       <c r="C611" t="inlineStr">
         <is>
-          <t>1. Да  
-2. Да</t>
+          <t>1. Да.  
+2. Да.</t>
         </is>
       </c>
     </row>
@@ -10410,7 +10408,7 @@
       </c>
       <c r="C614" t="inlineStr">
         <is>
-          <t>1. Нет.  
+          <t>1. Нет.
 2. Нет.</t>
         </is>
       </c>
@@ -10426,8 +10424,7 @@
       </c>
       <c r="C615" t="inlineStr">
         <is>
-          <t>1. Нет.
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -10680,8 +10677,7 @@
       </c>
       <c r="C631" t="inlineStr">
         <is>
-          <t>1. Нет.  
-2. Нет.</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>
@@ -11026,7 +11022,7 @@
       </c>
       <c r="C653" t="inlineStr">
         <is>
-          <t>Rate-limit error</t>
+          <t>Нет.</t>
         </is>
       </c>
     </row>

</xml_diff>